<commit_message>
correct mmrsurv equation (sign)
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/swm6_st-andrews_ac_uk/Documents/Projects/Global Health/gcrf2020/grade-DOH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swm6\OneDrive - University of St Andrews\Projects\Global Health\gcrf2020\grade-DOH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C72ECAEA-EDBC-4D2B-ACF6-80C9DCFBC443}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{50E4F672-CA8F-4354-A302-5BCB57E19DE4}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
+    <workbookView xWindow="4455" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E3CEA5-C44B-4D44-8DCE-3A5D6CE4EF75}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,16 @@
         <v>40</v>
       </c>
       <c r="E4" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42.060589412729861</v>
+      </c>
+      <c r="J4" s="1">
+        <v>59.805837819685323</v>
+      </c>
+      <c r="K4" s="1">
+        <v>47.343431044127705</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -636,7 +645,13 @@
         <v>1100</v>
       </c>
       <c r="E7" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>66.263254198720958</v>
+      </c>
+      <c r="N7" s="1">
+        <v>66.265000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -699,7 +714,16 @@
         <v>1200</v>
       </c>
       <c r="E10" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>99.206287487457246</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42.668358791697457</v>
+      </c>
+      <c r="N10" s="1">
+        <v>42.670999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -762,7 +786,13 @@
         <v>1200</v>
       </c>
       <c r="E13" s="1">
-        <v>0.5</v>
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>93.772924571552139</v>
+      </c>
+      <c r="M13" s="1">
+        <v>99.903619964787666</v>
       </c>
     </row>
   </sheetData>
@@ -772,6 +802,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002906F0B0D1A69B4397013659D63D4ECD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e94d17af6acb7c85dc4983b2f657d047">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e13dbb3c-56f9-4cde-a090-30dd7e47c75b" xmlns:ns4="24cc4736-4c37-4a3e-90b9-60f2bffa73c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9de179601fddb76822818ef21cf6ca6a" ns3:_="" ns4:_="">
     <xsd:import namespace="e13dbb3c-56f9-4cde-a090-30dd7e47c75b"/>
@@ -994,22 +1039,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FF61343-57DF-412E-AE7B-58BC50E79FE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1026,21 +1073,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
working version prior to changes to data source
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swm6\OneDrive - University of St Andrews\Projects\Global Health\gcrf2020\grade-DOH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{50E4F672-CA8F-4354-A302-5BCB57E19DE4}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C1CF070-69A1-41A3-B520-CBCE385F2D6B}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,9 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +454,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +472,7 @@
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -506,7 +515,7 @@
       <c r="M1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -561,6 +570,7 @@
       <c r="K3" s="1">
         <v>45.871220596898858</v>
       </c>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -587,6 +597,7 @@
       <c r="K4" s="1">
         <v>47.343431044127705</v>
       </c>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -627,7 +638,7 @@
       <c r="G6" s="1">
         <v>65.027598620552467</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="3">
         <v>65.028999999999996</v>
       </c>
     </row>
@@ -650,7 +661,7 @@
       <c r="G7" s="1">
         <v>66.263254198720958</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="3">
         <v>66.265000000000001</v>
       </c>
     </row>
@@ -699,6 +710,7 @@
       <c r="I9" s="1">
         <v>40.019954055617625</v>
       </c>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -722,7 +734,7 @@
       <c r="I10" s="1">
         <v>42.668358791697457</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="3">
         <v>42.670999999999999</v>
       </c>
     </row>
@@ -771,6 +783,7 @@
       <c r="M12" s="1">
         <v>99.891639430090351</v>
       </c>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -794,6 +807,7 @@
       <c r="M13" s="1">
         <v>99.903619964787666</v>
       </c>
+      <c r="N13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -802,21 +816,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002906F0B0D1A69B4397013659D63D4ECD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e94d17af6acb7c85dc4983b2f657d047">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e13dbb3c-56f9-4cde-a090-30dd7e47c75b" xmlns:ns4="24cc4736-4c37-4a3e-90b9-60f2bffa73c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9de179601fddb76822818ef21cf6ca6a" ns3:_="" ns4:_="">
     <xsd:import namespace="e13dbb3c-56f9-4cde-a090-30dd7e47c75b"/>
@@ -1039,24 +1038,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FF61343-57DF-412E-AE7B-58BC50E79FE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1073,4 +1070,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
parsed data stored as nested array via d3.nest rather than map
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swm6\OneDrive - University of St Andrews\Projects\Global Health\gcrf2020\grade-DOH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C1CF070-69A1-41A3-B520-CBCE385F2D6B}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{677D733E-EDC2-4CFD-864D-0EFB2FD40D63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2668F1FF-37FA-4835-8950-DE709290AD0A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{64988584-758D-49E9-87BD-96C0BDE181CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="comparison with tool and data" sheetId="1" r:id="rId1"/>
+    <sheet name="BASE data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>country</t>
   </si>
@@ -453,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E3CEA5-C44B-4D44-8DCE-3A5D6CE4EF75}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +816,373 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2A4979-45A7-4015-BD25-53018A0ACD66}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2006</v>
+      </c>
+      <c r="C2">
+        <v>32.756999999999998</v>
+      </c>
+      <c r="D2">
+        <v>32.756999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>38.406399999999998</v>
+      </c>
+      <c r="J2">
+        <v>58</v>
+      </c>
+      <c r="K2">
+        <v>45.866</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32.756999999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38.414000000000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>45.871000000000002</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2006</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32.756999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42.061</v>
+      </c>
+      <c r="K4" s="1">
+        <v>47.341999999999999</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>2011</v>
+      </c>
+      <c r="C5">
+        <v>1006.174</v>
+      </c>
+      <c r="D5">
+        <v>1047.3499999999999</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>63.929099999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2011</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1006.174</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>64.546000000000006</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2011</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1006.174</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>65.781000000000006</v>
+      </c>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2016</v>
+      </c>
+      <c r="C8">
+        <v>1136.681</v>
+      </c>
+      <c r="D8">
+        <v>1190.3599999999999</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>97.704899999999995</v>
+      </c>
+      <c r="I8">
+        <v>39.847999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1136.681</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>97.846999999999994</v>
+      </c>
+      <c r="I9" s="1">
+        <v>39.874000000000002</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1136.681</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>98.36</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42.524000000000001</v>
+      </c>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>2017</v>
+      </c>
+      <c r="C11">
+        <v>557.8845</v>
+      </c>
+      <c r="D11">
+        <v>595.41</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>91.94</v>
+      </c>
+      <c r="M11">
+        <v>99.759</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C12" s="1">
+        <v>557.8845</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>93.466999999999999</v>
+      </c>
+      <c r="M12" s="1">
+        <v>99.881</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C13" s="1">
+        <v>557.8845</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>93.643000000000001</v>
+      </c>
+      <c r="M13" s="1">
+        <v>99.893000000000001</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002906F0B0D1A69B4397013659D63D4ECD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e94d17af6acb7c85dc4983b2f657d047">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e13dbb3c-56f9-4cde-a090-30dd7e47c75b" xmlns:ns4="24cc4736-4c37-4a3e-90b9-60f2bffa73c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9de179601fddb76822818ef21cf6ca6a" ns3:_="" ns4:_="">
     <xsd:import namespace="e13dbb3c-56f9-4cde-a090-30dd7e47c75b"/>
@@ -1038,22 +1405,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FF61343-57DF-412E-AE7B-58BC50E79FE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1070,21 +1439,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666DEAC5-E7A3-40CF-8658-39B4611DDAAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE4EDEA4-51F9-403B-87A8-12DDD5A1A6A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>